<commit_message>
Incorporated files sent by WRI 6/29/20
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
+++ b/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
@@ -13,9 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="3" r:id="rId2"/>
-    <sheet name="GDPGR-alternate" sheetId="2" r:id="rId3"/>
-    <sheet name="GDPGR-bau" sheetId="8" r:id="rId4"/>
+    <sheet name="GDPGR-alternate" sheetId="2" r:id="rId2"/>
+    <sheet name="GDPGR-bau" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>About</t>
   </si>
@@ -129,9 +128,6 @@
     <t>Sources:</t>
   </si>
   <si>
-    <t>U.S. GDP Impact of SARC-CoV-2 Pandemic</t>
-  </si>
-  <si>
     <t>As of EPS 2.1.1, AEBC is set up to model the impacts of the 2020</t>
   </si>
   <si>
@@ -201,64 +197,32 @@
     <t>same year.</t>
   </si>
   <si>
-    <t>GDP Impact</t>
-  </si>
-  <si>
-    <t>January STEO</t>
-  </si>
-  <si>
-    <t>Source: Tables 9a, row 1</t>
-  </si>
-  <si>
-    <t>May STEO</t>
-  </si>
-  <si>
-    <t>Counterfactual GDP Growth Rate</t>
-  </si>
-  <si>
-    <t>GDP Growth Relative to Counterfactual Growth</t>
-  </si>
-  <si>
-    <t>2020 GDP Prediction</t>
-  </si>
-  <si>
-    <t>January STEO - Adjusted for 2019 value</t>
-  </si>
-  <si>
-    <t>U.S. Energy Information Administration</t>
-  </si>
-  <si>
-    <t>Short-Term Energy Outlook</t>
-  </si>
-  <si>
-    <t>https://www.eia.gov/outlooks/steo/</t>
-  </si>
-  <si>
-    <t>January 2020 and May 2020</t>
-  </si>
-  <si>
-    <t>Table 9a</t>
-  </si>
-  <si>
     <t>As of EPS 2.1.1, this variable is set up to model the impacts of the 2020</t>
   </si>
   <si>
-    <t>SARS-CoV-2 pandemic.  It uses the latest data available as of May 12,</t>
-  </si>
-  <si>
-    <t>Real GDP (billion chained 2012 dollars)</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARS-CoV-2 pandemic. </t>
+  </si>
+  <si>
+    <t>*This feature is not used in the Brazil EPS. However, users can customize</t>
+  </si>
+  <si>
+    <t>recession assumptions using this file, FoPITY (as explained below), and</t>
+  </si>
+  <si>
+    <t>EoSEUwGDPiR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="0.0000000000"/>
+  <numFmts count="1">
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,13 +239,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <u/>
       <sz val="11"/>
@@ -291,14 +248,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,50 +294,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -657,9 +596,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -668,162 +609,165 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="12"/>
+    </row>
+    <row r="6" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="8"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B6" s="21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B8" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="2"/>
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>39</v>
-      </c>
+      <c r="A33" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="7"/>
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
@@ -833,287 +777,69 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>9</v>
-      </c>
+      <c r="A75" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75" s="2"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A78" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B78" s="2"/>
+      <c r="A78" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="17.59765625" customWidth="1"/>
-    <col min="2" max="2" width="27.3984375" customWidth="1"/>
-    <col min="3" max="3" width="17.265625" customWidth="1"/>
-    <col min="4" max="7" width="8.73046875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B2">
-        <v>2019</v>
-      </c>
-      <c r="C2">
-        <v>2020</v>
-      </c>
-      <c r="D2">
-        <v>2021</v>
-      </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3">
-        <v>19073</v>
-      </c>
-      <c r="C3">
-        <v>18044</v>
-      </c>
-      <c r="D3">
-        <v>19194</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4">
-        <v>19068</v>
-      </c>
-      <c r="C4">
-        <v>19448</v>
-      </c>
-      <c r="D4">
-        <v>19790</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5">
-        <f>B3</f>
-        <v>19073</v>
-      </c>
-      <c r="C5" s="20">
-        <f>C4*($B$3/$B$4)</f>
-        <v>19453.099643381582</v>
-      </c>
-      <c r="D5" s="20">
-        <f>D4*($B$3/$B$4)</f>
-        <v>19795.189322425005</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="D7" s="12"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="5">
-        <f>(C3-C5)/C5</f>
-        <v>-7.2435738736422492E-2</v>
-      </c>
-      <c r="D8" s="5">
-        <f>(D3-D5)/D5</f>
-        <v>-3.0370476009741777E-2</v>
-      </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-    </row>
-    <row r="11" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="12">
-        <f>C5/B5-1</f>
-        <v>1.9928676316341543E-2</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="12">
-        <f>C3/B3-1</f>
-        <v>-5.3950610811094202E-2</v>
-      </c>
-      <c r="C12" s="15"/>
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1121,7 +847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -1138,20 +864,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>28</v>
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="22">
-        <f>Data!B11</f>
-        <v>1.9928676316341543E-2</v>
+        <v>26</v>
+      </c>
+      <c r="B2" s="9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -1167,7 +892,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1176,20 +901,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>28</v>
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="22">
-        <f>Data!B11</f>
-        <v>1.9928676316341543E-2</v>
+        <v>28</v>
+      </c>
+      <c r="B2" s="9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>